<commit_message>
- Base opt plots.
</commit_message>
<xml_diff>
--- a/src/output/opt/C_beta/data.xlsx
+++ b/src/output/opt/C_beta/data.xlsx
@@ -92,31 +92,31 @@
         <v>10</v>
       </c>
       <c r="F1" s="0">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="G1" s="0">
-        <v>1</v>
+        <v>0.90000000000000002</v>
       </c>
       <c r="H1" s="0">
         <v>10</v>
       </c>
       <c r="I1" s="0">
-        <v>209</v>
+        <v>269</v>
       </c>
       <c r="J1" s="0">
-        <v>5.4633906999999997</v>
+        <v>203.72656280000001</v>
       </c>
       <c r="K1" s="0">
-        <v>0.0039697926844040055</v>
+        <v>0.00060749954121108729</v>
       </c>
       <c r="L1" s="0">
-        <v>6.9395229595326809e-05</v>
+        <v>1.7457674885589531e-05</v>
       </c>
       <c r="M1" s="0">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N1" s="0">
-        <v>0</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2">

</xml_diff>